<commit_message>
adjusted excel sheet, added completion column
</commit_message>
<xml_diff>
--- a/work-breakdown-structure.xlsx
+++ b/work-breakdown-structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10110"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Marcy_Student/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Marcy_Student/Desktop/Marcy-Modules/CID/CID_data-slayer-corps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A370C916-F7BA-0048-8AB2-CC3EBF2F6608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDDC2F11-226D-9447-84BC-EC5C3322F73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4180" yWindow="760" windowWidth="24460" windowHeight="18360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="22" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
   <si>
     <t>1)</t>
   </si>
@@ -210,6 +210,15 @@
   </si>
   <si>
     <t>Phase 4</t>
+  </si>
+  <si>
+    <t>Completed?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Not Started</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1022,14 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1563,7 +1579,7 @@
   <dimension ref="B1:K30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1575,8 +1591,7 @@
     <col min="5" max="5" width="20" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="36.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="2" style="1" customWidth="1"/>
+    <col min="8" max="9" width="36.33203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="7.33203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="24.33203125" style="1" customWidth="1"/>
     <col min="12" max="16384" width="3.83203125" style="1"/>
@@ -1593,6 +1608,7 @@
       <c r="H1" s="41" t="s">
         <v>43</v>
       </c>
+      <c r="I1" s="41"/>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="2:11" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -1611,6 +1627,7 @@
       </c>
       <c r="E3" s="48"/>
       <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
       <c r="K3" s="67" t="s">
         <v>14</v>
       </c>
@@ -1619,6 +1636,7 @@
       <c r="D4" s="37"/>
       <c r="E4" s="37"/>
       <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
       <c r="J4" s="3"/>
       <c r="K4" s="4"/>
     </row>
@@ -1644,6 +1662,9 @@
       <c r="H5" s="62" t="s">
         <v>35</v>
       </c>
+      <c r="I5" s="62" t="s">
+        <v>55</v>
+      </c>
       <c r="K5" s="32"/>
     </row>
     <row r="6" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
@@ -1669,6 +1690,9 @@
       <c r="H6" s="77" t="s">
         <v>46</v>
       </c>
+      <c r="I6" s="77" t="s">
+        <v>56</v>
+      </c>
       <c r="K6" s="63"/>
     </row>
     <row r="7" spans="2:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
@@ -1694,6 +1718,9 @@
       <c r="H7" s="76" t="s">
         <v>48</v>
       </c>
+      <c r="I7" s="76" t="s">
+        <v>56</v>
+      </c>
       <c r="K7" s="34"/>
     </row>
     <row r="8" spans="2:11" ht="35" customHeight="1" x14ac:dyDescent="0.15">
@@ -1719,6 +1746,9 @@
       <c r="H8" s="74" t="s">
         <v>50</v>
       </c>
+      <c r="I8" s="74" t="s">
+        <v>56</v>
+      </c>
       <c r="K8" s="34"/>
     </row>
     <row r="9" spans="2:11" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -1742,6 +1772,9 @@
         <v>46036</v>
       </c>
       <c r="H9" s="70"/>
+      <c r="I9" s="70" t="s">
+        <v>57</v>
+      </c>
       <c r="K9" s="33"/>
     </row>
     <row r="10" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
@@ -1759,6 +1792,7 @@
       <c r="F10" s="68"/>
       <c r="G10" s="68"/>
       <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
       <c r="K10" s="33"/>
     </row>
     <row r="11" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
@@ -1777,6 +1811,7 @@
       <c r="F11" s="68"/>
       <c r="G11" s="68"/>
       <c r="H11" s="70"/>
+      <c r="I11" s="70"/>
       <c r="K11" s="33"/>
     </row>
     <row r="12" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
@@ -1795,6 +1830,7 @@
       <c r="F12" s="68"/>
       <c r="G12" s="68"/>
       <c r="H12" s="70"/>
+      <c r="I12" s="70"/>
       <c r="K12" s="33"/>
     </row>
     <row r="13" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
@@ -1813,6 +1849,7 @@
       <c r="F13" s="68"/>
       <c r="G13" s="68"/>
       <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
       <c r="K13" s="33"/>
     </row>
     <row r="14" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
@@ -1830,6 +1867,7 @@
       <c r="F14" s="68"/>
       <c r="G14" s="68"/>
       <c r="H14" s="70"/>
+      <c r="I14" s="70"/>
       <c r="K14" s="33"/>
     </row>
     <row r="15" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
@@ -1848,6 +1886,7 @@
       <c r="F15" s="68"/>
       <c r="G15" s="68"/>
       <c r="H15" s="70"/>
+      <c r="I15" s="70"/>
       <c r="K15" s="33"/>
     </row>
     <row r="16" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
@@ -1866,6 +1905,7 @@
       <c r="F16" s="68"/>
       <c r="G16" s="68"/>
       <c r="H16" s="70"/>
+      <c r="I16" s="70"/>
       <c r="K16" s="33"/>
     </row>
     <row r="17" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
@@ -1884,6 +1924,7 @@
       <c r="F17" s="68"/>
       <c r="G17" s="68"/>
       <c r="H17" s="70"/>
+      <c r="I17" s="70"/>
       <c r="K17" s="33"/>
     </row>
     <row r="18" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
@@ -1901,6 +1942,7 @@
       <c r="F18" s="68"/>
       <c r="G18" s="68"/>
       <c r="H18" s="70"/>
+      <c r="I18" s="70"/>
       <c r="K18" s="33"/>
     </row>
     <row r="19" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
@@ -1919,6 +1961,7 @@
       <c r="F19" s="68"/>
       <c r="G19" s="68"/>
       <c r="H19" s="70"/>
+      <c r="I19" s="70"/>
       <c r="K19" s="33"/>
     </row>
     <row r="20" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
@@ -1937,6 +1980,7 @@
       <c r="F20" s="68"/>
       <c r="G20" s="68"/>
       <c r="H20" s="70"/>
+      <c r="I20" s="70"/>
     </row>
     <row r="21" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="56">
@@ -1954,6 +1998,7 @@
       <c r="F21" s="68"/>
       <c r="G21" s="68"/>
       <c r="H21" s="70"/>
+      <c r="I21" s="70"/>
     </row>
     <row r="22" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="56">
@@ -1971,6 +2016,7 @@
       <c r="F22" s="68"/>
       <c r="G22" s="68"/>
       <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
     </row>
     <row r="23" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="56"/>
@@ -1983,6 +2029,7 @@
       <c r="F23" s="68"/>
       <c r="G23" s="68"/>
       <c r="H23" s="70"/>
+      <c r="I23" s="70"/>
     </row>
     <row r="24" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="56"/>
@@ -1995,6 +2042,7 @@
       <c r="F24" s="68"/>
       <c r="G24" s="68"/>
       <c r="H24" s="70"/>
+      <c r="I24" s="70"/>
     </row>
     <row r="25" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="56"/>
@@ -2007,6 +2055,7 @@
       <c r="F25" s="68"/>
       <c r="G25" s="68"/>
       <c r="H25" s="70"/>
+      <c r="I25" s="70"/>
     </row>
     <row r="26" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="56"/>
@@ -2019,6 +2068,7 @@
       <c r="F26" s="68"/>
       <c r="G26" s="68"/>
       <c r="H26" s="70"/>
+      <c r="I26" s="70"/>
     </row>
     <row r="27" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="56"/>
@@ -2031,6 +2081,7 @@
       <c r="F27" s="68"/>
       <c r="G27" s="68"/>
       <c r="H27" s="70"/>
+      <c r="I27" s="70"/>
     </row>
     <row r="28" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="56"/>
@@ -2043,6 +2094,7 @@
       <c r="F28" s="68"/>
       <c r="G28" s="68"/>
       <c r="H28" s="70"/>
+      <c r="I28" s="70"/>
     </row>
     <row r="29" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="64"/>
@@ -2055,6 +2107,7 @@
       <c r="F29" s="69"/>
       <c r="G29" s="69"/>
       <c r="H29" s="71"/>
+      <c r="I29" s="71"/>
     </row>
     <row r="30" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K30" s="63" t="s">
@@ -2063,6 +2116,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:E9 H6:H9 B10:H29">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>($B6=1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6:I29">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>($B6=1)</formula>
     </cfRule>

</xml_diff>